<commit_message>
gitignore update, prototype 1, logboek
</commit_message>
<xml_diff>
--- a/documentation/logboek/logboek.xlsx
+++ b/documentation/logboek/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerbe\GLU\Git\WeBuilders\documentation\logboek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerbe\GLU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60BBF1-78A6-48FD-A6AB-20B2FF3FE18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1035E7-7A6B-4810-AFA7-281D6FB869DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gerben" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Dag</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>Websites analyseren, wireframes en sitemap maken</t>
+  </si>
+  <si>
+    <t>Werken aan home page prototype 1</t>
+  </si>
+  <si>
+    <t>Gewerkt aan prototype 3</t>
+  </si>
+  <si>
+    <t>Gewerkt aan prototype 2</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -458,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,43 +541,53 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="B6" s="6">
         <v>44883</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.59375</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="11">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <v>0.67708333333333337</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="10">
+        <v>44886</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
@@ -705,7 +724,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,43 +797,53 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="B6" s="6">
         <v>44883</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.59375</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="11">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <v>0.67708333333333337</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="10">
+        <v>44886</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
@@ -950,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4180284E-C559-42C2-A5F1-1D235DA9BAD4}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,43 +1053,53 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="B6" s="6">
         <v>44883</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>0.59375</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="11">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <v>0.67708333333333337</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="10">
+        <v>44886</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>

</xml_diff>